<commit_message>
ACFP-1033 Grant read access on TASK to assignee and collaborator group
</commit_message>
<xml_diff>
--- a/acm/acm-config-server-repo/rules/drools-access-control-rules.xlsx
+++ b/acm/acm-config-server-repo/rules/drools-access-control-rules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleksandar.acevski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D5AF28-FEB8-4C96-99C1-7B375A6A672B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{98E91FD3-78A5-417F-8F51-31792AC90C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,17 @@
     <definedName name="ObjectTypes">Sheet2!$A$2:$A$51</definedName>
     <definedName name="ParticipantTypes">Sheet2!$B$2:$B$51</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -31,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="164">
   <si>
     <t>RuleSet</t>
   </si>
@@ -171,21 +180,33 @@
     <t>Complaint – Only participants can add files</t>
   </si>
   <si>
+    <t>grant add file to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
     <t>Complaint – Only participants can save</t>
   </si>
   <si>
+    <t>grant save to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
     <t>Complaint – Everyone can upload or replace files</t>
   </si>
   <si>
     <t>status != 'CLOSED' &amp;&amp; status != 'DELETE' &amp;&amp; status != 'DELETED'</t>
   </si>
   <si>
+    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower,  *</t>
+  </si>
+  <si>
     <t>Complaint – Deny upload or replace files on closed complaint</t>
   </si>
   <si>
     <t>status == 'CLOSED' || status == 'DELETE' || status == 'DELETED'</t>
   </si>
   <si>
+    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower, *</t>
+  </si>
+  <si>
     <t>Complaint – Anybody can add comments</t>
   </si>
   <si>
@@ -204,6 +225,15 @@
     <t>grant addTag to *</t>
   </si>
   <si>
+    <t>Complaint – Restricted Flag</t>
+  </si>
+  <si>
+    <t>restricted</t>
+  </si>
+  <si>
+    <t>deny read to *</t>
+  </si>
+  <si>
     <t>Case File – Assignee Read Access</t>
   </si>
   <si>
@@ -213,6 +243,9 @@
     <t>Case File – Grant Participants Access to Drafts</t>
   </si>
   <si>
+    <t>grant read to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, follower, reader</t>
+  </si>
+  <si>
     <t>Case File – Grant Access to non-Drafts</t>
   </si>
   <si>
@@ -231,13 +264,7 @@
     <t>status == 'DELETED'</t>
   </si>
   <si>
-    <t>Complaint – Restricted Flag</t>
-  </si>
-  <si>
-    <t>restricted</t>
-  </si>
-  <si>
-    <t>deny read to *</t>
+    <t>mandatory deny read to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, *</t>
   </si>
   <si>
     <t>Case File – Restricted Flag</t>
@@ -246,27 +273,87 @@
     <t>Case File – Only participants can view details page</t>
   </si>
   <si>
+    <t>grant viewCaseDetailsPage to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
+  </si>
+  <si>
+    <t>grant saveCase to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
     <t>Case File – Everyone can upload or replace files</t>
   </si>
   <si>
+    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower, *</t>
+  </si>
+  <si>
     <t>Case File –  Deny upload or replace files on closed case file</t>
   </si>
   <si>
     <t>Case File – Only participants can add comments</t>
   </si>
   <si>
+    <t>grant addComment to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
+  </si>
+  <si>
     <t>Case File – anyone can subscribe</t>
   </si>
   <si>
     <t>Case File – anyone can add tag</t>
   </si>
   <si>
+    <t>Consultation – Assignee Read Access</t>
+  </si>
+  <si>
+    <t>CONSULTATION</t>
+  </si>
+  <si>
+    <t>Consultation – Grant Participants Access to Drafts</t>
+  </si>
+  <si>
+    <t>Consultation – Grant Access to non-Drafts</t>
+  </si>
+  <si>
+    <t>Consultation – Lockout No Access Users</t>
+  </si>
+  <si>
+    <t>Consultation – Only participants can add files</t>
+  </si>
+  <si>
+    <t>Consultation – Only participants can save</t>
+  </si>
+  <si>
+    <t>Consultation – Deleted Cases</t>
+  </si>
+  <si>
+    <t>Consultation – Restricted Flag</t>
+  </si>
+  <si>
+    <t>Consultation – Only participants can view details page</t>
+  </si>
+  <si>
+    <t>Consultation – Everyone can upload or replace files</t>
+  </si>
+  <si>
+    <t>Consultation –  Deny upload or replace files on closed Consultation</t>
+  </si>
+  <si>
+    <t>Consultation – Only participants can add comments</t>
+  </si>
+  <si>
+    <t>Consultation – anyone can subscribe</t>
+  </si>
+  <si>
+    <t>Consultation – anyone can add tag</t>
+  </si>
+  <si>
     <t>Task – default read access</t>
   </si>
   <si>
     <t>TASK</t>
   </si>
   <si>
+    <t>grant read to *, assignee, owning group, collaborator group</t>
+  </si>
+  <si>
     <t>Task – Only participants can add files</t>
   </si>
   <si>
@@ -303,6 +390,9 @@
     <t>Task – Only participants can add tags</t>
   </si>
   <si>
+    <t>grant addTag to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
+  </si>
+  <si>
     <t>Folder - default list folder</t>
   </si>
   <si>
@@ -348,6 +438,9 @@
     <t>DOC_REPO</t>
   </si>
   <si>
+    <t>grant read to owner, owning group, collaborator group, collaborator, reader, *</t>
+  </si>
+  <si>
     <t>DocumentRepository – Anybody can add comments</t>
   </si>
   <si>
@@ -366,9 +459,18 @@
     <t>DocumentRepository – Everyone can upload or replace files</t>
   </si>
   <si>
+    <t>grant add file to owner, owning group, collaborator group, collaborator, *</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to  owner, owning group, collaborator group, collaborator, *</t>
+  </si>
+  <si>
     <t>DocumentRepository – Only participants can save</t>
   </si>
   <si>
+    <t>grant save to owner, owning group, collaborator group, collaborator</t>
+  </si>
+  <si>
     <t>Organization – Lockout No Access Users</t>
   </si>
   <si>
@@ -399,6 +501,36 @@
     <t>Person – Restricted Flag</t>
   </si>
   <si>
+    <t>Costsheet – default read access</t>
+  </si>
+  <si>
+    <t>COSTSHEET</t>
+  </si>
+  <si>
+    <t>Costsheet – Only participants can add files</t>
+  </si>
+  <si>
+    <t>grant add file to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>Costsheet – Only participants can save</t>
+  </si>
+  <si>
+    <t>grant save to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>Costsheet –  Only participants can upload or replace files</t>
+  </si>
+  <si>
+    <t>grant uploadOrReplaceFile to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
+  </si>
+  <si>
+    <t>BusinessProcess – Grant Access</t>
+  </si>
+  <si>
+    <t>BUSINESS_PROCESS</t>
+  </si>
+  <si>
     <t>Object Types</t>
   </si>
   <si>
@@ -415,126 +547,6 @@
   </si>
   <si>
     <t>ACCESS CONTROL LIST</t>
-  </si>
-  <si>
-    <t>Costsheet – Only participants can add files</t>
-  </si>
-  <si>
-    <t>COSTSHEET</t>
-  </si>
-  <si>
-    <t>Costsheet – default read access</t>
-  </si>
-  <si>
-    <t>Costsheet – Only participants can save</t>
-  </si>
-  <si>
-    <t>Costsheet –  Only participants can upload or replace files</t>
-  </si>
-  <si>
-    <t>BUSINESS_PROCESS</t>
-  </si>
-  <si>
-    <t>BusinessProcess – Grant Access</t>
-  </si>
-  <si>
-    <t>grant add file to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
-  </si>
-  <si>
-    <t>grant save to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
-  </si>
-  <si>
-    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower,  *</t>
-  </si>
-  <si>
-    <t>deny uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower, *</t>
-  </si>
-  <si>
-    <t>grant read to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, follower, reader</t>
-  </si>
-  <si>
-    <t>mandatory deny read to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, *</t>
-  </si>
-  <si>
-    <t>grant viewCaseDetailsPage to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
-  </si>
-  <si>
-    <t>grant saveCase to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
-  </si>
-  <si>
-    <t>grant uploadOrReplaceFile to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader, follower, *</t>
-  </si>
-  <si>
-    <t>grant addComment to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
-  </si>
-  <si>
-    <t>grant addTag to assignee, co-owner, supervisor, owning group, collaborator group, approver, collaborator, reader</t>
-  </si>
-  <si>
-    <t>grant read to owner, owning group, collaborator group, collaborator, reader, *</t>
-  </si>
-  <si>
-    <t>grant add file to owner, owning group, collaborator group, collaborator, *</t>
-  </si>
-  <si>
-    <t>grant uploadOrReplaceFile to  owner, owning group, collaborator group, collaborator, *</t>
-  </si>
-  <si>
-    <t>grant save to owner, owning group, collaborator group, collaborator</t>
-  </si>
-  <si>
-    <t>grant add file to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
-  </si>
-  <si>
-    <t>grant save to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
-  </si>
-  <si>
-    <t>grant uploadOrReplaceFile to assignee, owner, co-owner, supervisor, owning group, collaborator group, approver, collaborator</t>
-  </si>
-  <si>
-    <t>Consultation – Assignee Read Access</t>
-  </si>
-  <si>
-    <t>Consultation – Grant Participants Access to Drafts</t>
-  </si>
-  <si>
-    <t>Consultation – Grant Access to non-Drafts</t>
-  </si>
-  <si>
-    <t>Consultation – Lockout No Access Users</t>
-  </si>
-  <si>
-    <t>Consultation – Only participants can add files</t>
-  </si>
-  <si>
-    <t>Consultation – Only participants can save</t>
-  </si>
-  <si>
-    <t>Consultation – Deleted Cases</t>
-  </si>
-  <si>
-    <t>Consultation – Restricted Flag</t>
-  </si>
-  <si>
-    <t>Consultation – Only participants can view details page</t>
-  </si>
-  <si>
-    <t>Consultation – Everyone can upload or replace files</t>
-  </si>
-  <si>
-    <t>Consultation –  Deny upload or replace files on closed Consultation</t>
-  </si>
-  <si>
-    <t>Consultation – Only participants can add comments</t>
-  </si>
-  <si>
-    <t>Consultation – anyone can subscribe</t>
-  </si>
-  <si>
-    <t>Consultation – anyone can add tag</t>
-  </si>
-  <si>
-    <t>CONSULTATION</t>
   </si>
 </sst>
 </file>
@@ -544,7 +556,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1191,23 +1203,23 @@
   </sheetPr>
   <dimension ref="A2:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" customWidth="1"/>
-    <col min="2" max="2" width="24.265625" customWidth="1"/>
-    <col min="3" max="3" width="49.86328125" customWidth="1"/>
-    <col min="4" max="4" width="36.1328125" customWidth="1"/>
-    <col min="5" max="5" width="43.86328125" customWidth="1"/>
-    <col min="6" max="6" width="30.59765625" customWidth="1"/>
-    <col min="7" max="7" width="35.59765625" customWidth="1"/>
-    <col min="8" max="1025" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="8" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1217,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -1227,7 +1239,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1237,7 +1249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1247,7 +1259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1257,7 +1269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1267,7 +1279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1277,7 +1289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1287,7 +1299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1297,7 +1309,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1307,7 +1319,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="327.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="327.75">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1317,7 +1329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
@@ -1327,7 +1339,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -1338,7 +1350,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1357,7 +1369,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="4" t="s">
@@ -1368,7 +1380,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
@@ -1387,7 +1399,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="85.5">
       <c r="A19" s="11" t="s">
         <v>23</v>
       </c>
@@ -1410,7 +1422,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="28.5">
       <c r="A20" s="1"/>
       <c r="B20" s="16" t="s">
         <v>30</v>
@@ -1425,7 +1437,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" ht="28.5">
       <c r="A21" s="1"/>
       <c r="B21" s="16" t="s">
         <v>33</v>
@@ -1442,7 +1454,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" ht="28.5">
       <c r="A22" s="1"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
@@ -1459,7 +1471,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" ht="28.5">
       <c r="A23" s="1"/>
       <c r="B23" s="16" t="s">
         <v>38</v>
@@ -1474,7 +1486,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" ht="42.75">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
@@ -1486,13 +1498,13 @@
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="42.75">
       <c r="A25" s="1"/>
       <c r="B25" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>31</v>
@@ -1501,47 +1513,47 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="57">
       <c r="A26" s="1"/>
       <c r="B26" s="16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="57">
       <c r="A27" s="1"/>
       <c r="B27" s="16" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.5">
       <c r="A28" s="1"/>
       <c r="B28" s="16" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>31</v>
@@ -1550,13 +1562,13 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.5">
       <c r="A29" s="1"/>
       <c r="B29" s="16" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>31</v>
@@ -1565,13 +1577,13 @@
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.5">
       <c r="A30" s="1"/>
       <c r="B30" s="16" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>31</v>
@@ -1580,33 +1592,33 @@
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1"/>
       <c r="B31" s="16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="28.5">
       <c r="A32" s="1"/>
       <c r="B32" s="16" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="18"/>
@@ -1615,13 +1627,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="57">
       <c r="A33" s="1"/>
       <c r="B33" s="16" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>34</v>
@@ -1629,16 +1641,16 @@
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="28.5">
       <c r="A34" s="1"/>
       <c r="B34" s="16" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>37</v>
@@ -1649,13 +1661,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="28.5">
       <c r="A35" s="1"/>
       <c r="B35" s="16" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -1664,186 +1676,186 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="42.75">
       <c r="A36" s="1"/>
       <c r="B36" s="16" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="42.75">
       <c r="A37" s="1"/>
       <c r="B37" s="16" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="57">
       <c r="A38" s="1"/>
       <c r="B38" s="16" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1"/>
       <c r="B39" s="16" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="57">
       <c r="A40" s="1"/>
       <c r="B40" s="16" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="42.75">
       <c r="A41" s="1"/>
       <c r="B41" s="16" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="57">
       <c r="A42" s="1"/>
       <c r="B42" s="16" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="57">
       <c r="A43" s="1"/>
       <c r="B43" s="16" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="42.75">
       <c r="A44" s="1"/>
       <c r="B44" s="16" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="28.5">
       <c r="A45" s="1"/>
       <c r="B45" s="16" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D45" s="17"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="28.5">
       <c r="A46" s="1"/>
       <c r="B46" s="16" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="28.5">
       <c r="A47" s="1"/>
       <c r="B47" s="16" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="18"/>
@@ -1852,13 +1864,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" ht="57">
       <c r="A48" s="1"/>
       <c r="B48" s="16" t="s">
-        <v>149</v>
+        <v>83</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>34</v>
@@ -1866,16 +1878,16 @@
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.5">
       <c r="A49" s="1"/>
       <c r="B49" s="16" t="s">
-        <v>150</v>
+        <v>84</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D49" s="17" t="s">
         <v>37</v>
@@ -1886,13 +1898,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" ht="28.5">
       <c r="A50" s="1"/>
       <c r="B50" s="16" t="s">
-        <v>151</v>
+        <v>85</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
@@ -1901,492 +1913,492 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" ht="42.75">
       <c r="A51" s="1"/>
       <c r="B51" s="16" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D51" s="17"/>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
       <c r="G51" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="42.75">
       <c r="A52" s="1"/>
       <c r="B52" s="16" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D52" s="17"/>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
       <c r="G52" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="57">
       <c r="A53" s="1"/>
       <c r="B53" s="16" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
       <c r="G53" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1"/>
       <c r="B54" s="16" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="57">
       <c r="A55" s="1"/>
       <c r="B55" s="16" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
       <c r="G55" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="42.75">
       <c r="A56" s="1"/>
       <c r="B56" s="16" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D56" s="17"/>
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
       <c r="G56" s="16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="57">
       <c r="A57" s="1"/>
       <c r="B57" s="16" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
       <c r="G57" s="16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="57">
       <c r="A58" s="1"/>
       <c r="B58" s="16" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E58" s="18"/>
       <c r="F58" s="18"/>
       <c r="G58" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="42.75">
       <c r="A59" s="1"/>
       <c r="B59" s="16" t="s">
-        <v>159</v>
+        <v>93</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D59" s="17"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18"/>
       <c r="G59" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="28.5">
       <c r="A60" s="1"/>
       <c r="B60" s="16" t="s">
-        <v>160</v>
+        <v>94</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D60" s="17"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
       <c r="G60" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="28.5">
       <c r="A61" s="1"/>
       <c r="B61" s="16" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="D61" s="17"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18"/>
       <c r="G61" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1"/>
       <c r="B62" s="16" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
       <c r="F62" s="18"/>
       <c r="G62" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="42.75">
       <c r="A63" s="1"/>
       <c r="B63" s="16" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D63" s="17"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
       <c r="G63" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="42.75">
       <c r="A64" s="1"/>
       <c r="B64" s="16" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D64" s="17"/>
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
       <c r="G64" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="28.5">
       <c r="A65" s="1"/>
       <c r="B65" s="16" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D65" s="17"/>
       <c r="E65" s="18"/>
       <c r="F65" s="18"/>
       <c r="G65" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="28.5">
       <c r="A66" s="1"/>
       <c r="B66" s="16" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D66" s="17"/>
       <c r="E66" s="18"/>
       <c r="F66" s="18"/>
       <c r="G66" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="57">
       <c r="A67" s="1"/>
       <c r="B67" s="16" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
       <c r="G67" s="16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="57">
       <c r="A68" s="1"/>
       <c r="B68" s="16" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E68" s="18"/>
       <c r="F68" s="18"/>
       <c r="G68" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="42.75">
       <c r="A69" s="1"/>
       <c r="B69" s="16" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D69" s="17"/>
       <c r="E69" s="18"/>
       <c r="F69" s="18"/>
       <c r="G69" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="1"/>
       <c r="B70" s="16" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D70" s="17"/>
       <c r="E70" s="18"/>
       <c r="F70" s="18"/>
       <c r="G70" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="42.75">
       <c r="A71" s="1"/>
       <c r="B71" s="16" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D71" s="17"/>
       <c r="E71" s="18"/>
       <c r="F71" s="18"/>
       <c r="G71" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="28.5">
       <c r="A72" s="1"/>
       <c r="B72" s="16" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D72" s="18"/>
       <c r="E72" s="18"/>
       <c r="F72" s="18"/>
       <c r="G72" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="17.25" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="16" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D73" s="18"/>
       <c r="E73" s="18"/>
       <c r="F73" s="18"/>
       <c r="G73" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="28.5">
       <c r="A74" s="1"/>
       <c r="B74" s="16" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D74" s="18"/>
       <c r="E74" s="18"/>
       <c r="F74" s="18"/>
       <c r="G74" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="1"/>
       <c r="B75" s="16" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E75" s="18"/>
       <c r="F75" s="18"/>
       <c r="G75" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="28.5">
       <c r="A76" s="1"/>
       <c r="B76" s="16" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="18"/>
       <c r="F76" s="18"/>
       <c r="G76" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="1"/>
       <c r="B77" s="16" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="18"/>
       <c r="F77" s="18"/>
       <c r="G77" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="28.5">
       <c r="A78" s="1"/>
       <c r="B78" s="16" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="D78" s="18"/>
       <c r="E78" s="18"/>
       <c r="F78" s="18"/>
       <c r="G78" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="1"/>
       <c r="B79" s="16" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E79" s="18"/>
       <c r="F79" s="18"/>
       <c r="G79" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="28.5">
       <c r="A80" s="1"/>
       <c r="B80" s="16" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D80" s="18"/>
       <c r="E80" s="18"/>
       <c r="F80" s="18"/>
       <c r="G80" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" ht="28.5">
       <c r="B81" s="16" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D81" s="16"/>
       <c r="E81" s="16"/>
       <c r="F81" s="16"/>
       <c r="G81" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="28.5">
       <c r="B82" s="16" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D82" s="16"/>
       <c r="E82" s="16"/>
@@ -2395,98 +2407,98 @@
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:7" ht="28.5">
       <c r="B83" s="16" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D83" s="16"/>
       <c r="E83" s="16"/>
       <c r="F83" s="16"/>
       <c r="G83" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" ht="28.5">
       <c r="B84" s="16" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D84" s="16"/>
       <c r="E84" s="16"/>
       <c r="F84" s="16"/>
       <c r="G84" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" ht="28.5">
       <c r="B85" s="16" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E85" s="18"/>
       <c r="F85" s="18"/>
       <c r="G85" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" ht="42.75">
       <c r="B86" s="16" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="C86" s="18" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D86" s="17"/>
       <c r="E86" s="18"/>
       <c r="F86" s="18"/>
       <c r="G86" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" ht="42.75">
       <c r="B87" s="16" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D87" s="17"/>
       <c r="E87" s="18"/>
       <c r="F87" s="18"/>
       <c r="G87" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" ht="28.5">
       <c r="B88" s="16" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D88" s="17"/>
       <c r="E88" s="18"/>
       <c r="F88" s="18"/>
       <c r="G88" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" ht="28.5">
       <c r="B89" s="16" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="D89" s="17"/>
       <c r="E89" s="18"/>
@@ -2495,56 +2507,56 @@
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:7" ht="28.5">
       <c r="B90" s="16" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="D90" s="17"/>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
       <c r="G90" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" ht="28.5">
+      <c r="B91" s="16" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="91" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B91" s="16" t="s">
-        <v>110</v>
-      </c>
       <c r="C91" s="17" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="D91" s="17"/>
       <c r="E91" s="18"/>
       <c r="F91" s="18"/>
       <c r="G91" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="28.5">
       <c r="B92" s="16" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="C92" s="18" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E92" s="18"/>
       <c r="F92" s="18"/>
       <c r="G92" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="28.5">
       <c r="B93" s="16" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D93" s="17"/>
       <c r="E93" s="18"/>
@@ -2553,57 +2565,57 @@
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:7" ht="28.5">
       <c r="B94" s="16" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D94" s="17"/>
       <c r="E94" s="18"/>
       <c r="F94" s="18"/>
       <c r="G94" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" ht="28.5">
       <c r="B95" s="16" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D95" s="17"/>
       <c r="E95" s="18"/>
       <c r="F95" s="18"/>
       <c r="G95" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7">
+      <c r="B96" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C96" s="17" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B96" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>113</v>
-      </c>
       <c r="D96" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E96" s="18"/>
       <c r="F96" s="18"/>
       <c r="G96" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="28.5">
       <c r="A97" s="1"/>
       <c r="B97" s="16" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="C97" s="18" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="D97" s="18"/>
       <c r="E97" s="18"/>
@@ -2612,57 +2624,57 @@
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" ht="42.75">
       <c r="A98" s="1"/>
       <c r="B98" s="16" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="D98" s="17"/>
       <c r="E98" s="18"/>
       <c r="F98" s="18"/>
       <c r="G98" s="16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="42.75">
       <c r="A99" s="1"/>
       <c r="B99" s="16" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="D99" s="17"/>
       <c r="E99" s="18"/>
       <c r="F99" s="18"/>
       <c r="G99" s="16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="57">
       <c r="A100" s="1"/>
       <c r="B100" s="16" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="C100" s="18" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="D100" s="20"/>
       <c r="E100" s="18"/>
       <c r="F100" s="18"/>
       <c r="G100" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="28.5">
       <c r="B101" s="16" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="D101" s="17"/>
       <c r="E101" s="18"/>
@@ -2688,50 +2700,50 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.73046875" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" customWidth="1"/>
-    <col min="3" max="1025" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2749,9 +2761,9 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>